<commit_message>
animations and dialogue update
</commit_message>
<xml_diff>
--- a/Incremental Demon Game Project/dialogue.xlsx
+++ b/Incremental Demon Game Project/dialogue.xlsx
@@ -1,34 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\incremental-demon-game\Incremental Demon Game Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86750F-33B5-4065-8D34-C5EEF9D41487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE94E845-F260-4047-AD1E-F56CA5367CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
-  <si>
-    <t>dialogue ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>speaker</t>
   </si>
@@ -76,16 +84,31 @@
   </si>
   <si>
     <t>scene ID</t>
+  </si>
+  <si>
+    <t>dialogue line ID</t>
+  </si>
+  <si>
+    <t>001OpeningScene</t>
+  </si>
+  <si>
+    <t>Line number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,151 +417,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="192.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="192.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(C2,B2,D2)</f>
+        <v>001OpeningScene1Kellavar</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A7" si="0">_xlfn.CONCAT(C3,B3,D3)</f>
+        <v>001OpeningScene2Kellavar</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>001OpeningScene3Kellavar</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>001OpeningScene4Kellavar</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>001OpeningScene5Kellavar</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>001OpeningScene6Kellavar</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>